<commit_message>
error report created by sen_validator class
</commit_message>
<xml_diff>
--- a/fake_data/fake_sen.xlsx
+++ b/fake_data/fake_sen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eschdata\Strategic_Resourcing_CS$\Performance Improvement Team\Data to Insight\Will\AnnexA SEN Validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5E31428-2A15-48FB-8B34-0AEF80CAA7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DD5898-3430-4493-8200-17F185E5CD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10780" activeTab="1" xr2:uid="{221BFC75-F63B-4D5C-A32E-B8E8FE19366A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{221BFC75-F63B-4D5C-A32E-B8E8FE19366A}"/>
   </bookViews>
   <sheets>
     <sheet name="List_1" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Unique ID</t>
   </si>
@@ -120,6 +120,51 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>wilbert</t>
+  </si>
+  <si>
+    <t>jnroasvn</t>
+  </si>
+  <si>
+    <t>mrv</t>
+  </si>
+  <si>
+    <t>WIRI</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>nutley</t>
+  </si>
+  <si>
+    <t>ayes</t>
+  </si>
+  <si>
+    <t>hmm</t>
+  </si>
+  <si>
+    <t>willis</t>
+  </si>
+  <si>
+    <t>dfnjfd</t>
+  </si>
+  <si>
+    <t>fjkndkj</t>
+  </si>
+  <si>
+    <t>WIRT</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Place 2</t>
   </si>
 </sst>
 </file>
@@ -202,7 +247,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -370,7 +415,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{A424023A-35C6-4884-B25A-7522B734B4C0}" name="List_2" displayName="List_2" ref="A1:Q2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{A424023A-35C6-4884-B25A-7522B734B4C0}" name="List_2" displayName="List_2" ref="A1:Q4" totalsRowShown="0">
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{98C25340-DCA5-495A-A513-051CD11916B3}" name="Unique ID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{89EB73FA-A7D8-478D-AAE9-1D59F69D8A85}" name="UPN" dataDxfId="4"/>
@@ -711,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FBD436-D28B-445A-8ADB-FE89B59F467D}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -860,6 +905,71 @@
         <v>31</v>
       </c>
     </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4">
+        <v>36892</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="5">
+        <v>38019</v>
+      </c>
+      <c r="H3" s="5">
+        <v>39969</v>
+      </c>
+      <c r="I3" s="5">
+        <v>40890</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -871,10 +981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{484F405A-046A-4D54-8DFB-8B05AE956DB7}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -994,6 +1104,62 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4">
+        <v>33216</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D4" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>